<commit_message>
Election.Analytic.System.v2 - PPRP  #612 - Implements MPDCOffifial #6
</commit_message>
<xml_diff>
--- a/Imports/Excels/10.ข้อมูลผู้สมัครรับเลือกตั้งสมาชิกสภาผู้แทนแบบแบ่งเขต อย่างเป็นทางการ ปี 2566_v8.xlsx
+++ b/Imports/Excels/10.ข้อมูลผู้สมัครรับเลือกตั้งสมาชิกสภาผู้แทนแบบแบ่งเขต อย่างเป็นทางการ ปี 2566_v8.xlsx
@@ -7355,9 +7355,6 @@
     <t>คุณ โกมินทร์ พิมพ์จันทร์</t>
   </si>
   <si>
-    <t>นาย ชานุวัฒน์ วรามิตร</t>
-  </si>
-  <si>
     <t>นาย ธงชัย นายกชน</t>
   </si>
   <si>
@@ -7365,6 +7362,9 @@
   </si>
   <si>
     <t>ลำดับ</t>
+  </si>
+  <si>
+    <t>นาย ชานุวัฒน์ วรามิตร</t>
   </si>
 </sst>
 </file>
@@ -7853,7 +7853,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7867,7 +7867,7 @@
   <dimension ref="A1:F2392"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
@@ -7892,7 +7892,7 @@
         <v>82</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>77</v>
@@ -7918,7 +7918,7 @@
         <v>79</v>
       </c>
       <c r="F2" s="6">
-        <v>6000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -7938,7 +7938,7 @@
         <v>80</v>
       </c>
       <c r="F3" s="6">
-        <v>5000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -17509,7 +17509,7 @@
         <v>5</v>
       </c>
       <c r="C482" s="13" t="s">
-        <v>2443</v>
+        <v>2446</v>
       </c>
       <c r="D482" s="7">
         <v>1</v>
@@ -23749,7 +23749,7 @@
         <v>2</v>
       </c>
       <c r="C794" s="13" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
       <c r="D794" s="7">
         <v>1</v>
@@ -25389,7 +25389,7 @@
         <v>4</v>
       </c>
       <c r="C876" s="13" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
       <c r="D876" s="7">
         <v>5</v>

</xml_diff>